<commit_message>
Finalizes RNAseq implementation. Adds ability ot reference fields from yaml assay config by number in addition to by name. Fixes a bug for loading date values from excel files.
</commit_message>
<xml_diff>
--- a/data_examples/J_Drive/ECHO/HIV/HI/PBMC/AssayData/RNAseq/DataQC/20191023_DARPA RNA samples  for mRNAseq.xlsx
+++ b/data_examples/J_Drive/ECHO/HIV/HI/PBMC/AssayData/RNAseq/DataQC/20191023_DARPA RNA samples  for mRNAseq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\Darpa\Programming\submission\data_examples\J_Drive\ECHO\HIV\HI\PBMC\AssayData\RNAseq\DataQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559D67D8-036D-45C4-8069-1A93575CEB5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06DCDA-7DAE-439A-9DD1-17ABE35E2302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hawaii PBMCs" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="176">
   <si>
     <t>A260/A280</t>
   </si>
@@ -102,21 +102,6 @@
     <t>Nanodrop</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">RNA conc </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ng/ul)</t>
-    </r>
-  </si>
-  <si>
     <t>AS15-06663_3</t>
   </si>
   <si>
@@ -565,6 +550,15 @@
   </si>
   <si>
     <t>AS14-00902_3</t>
+  </si>
+  <si>
+    <t>Bioanalyzer/RNA conc (ng/ul)</t>
+  </si>
+  <si>
+    <t>Picogreen/RNA conc (ng/ul)</t>
+  </si>
+  <si>
+    <t>Nanodrop/RNA conc (ng/ul)</t>
   </si>
 </sst>
 </file>
@@ -1219,45 +1213,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.90625" style="4"/>
+    <col min="1" max="1" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="4"/>
     <col min="8" max="8" width="10" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.90625" style="4"/>
-    <col min="10" max="10" width="8.90625" style="23"/>
-    <col min="11" max="11" width="11.54296875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="12.54296875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="23"/>
+    <col min="11" max="11" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="4" customWidth="1"/>
     <col min="15" max="15" width="10" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.90625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="13.08984375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.453125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="4" customWidth="1"/>
     <col min="19" max="19" width="12" style="4" customWidth="1"/>
-    <col min="20" max="16384" width="8.90625" style="4"/>
+    <col min="20" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
@@ -1276,7 +1270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
@@ -1287,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>23</v>
+        <v>175</v>
       </c>
       <c r="E4" s="36" t="s">
         <v>0</v>
@@ -1302,43 +1296,43 @@
         <v>20</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>23</v>
+        <v>173</v>
       </c>
       <c r="J4" s="30" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>23</v>
+        <v>174</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="O4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="S4" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="S4" s="14" t="s">
+      <c r="T4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>1</v>
       </c>
@@ -1346,7 +1340,7 @@
         <v>43676</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="12">
         <v>19.100000000000001</v>
@@ -1377,7 +1371,7 @@
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>2</v>
       </c>
@@ -1385,7 +1379,7 @@
         <v>43676</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D6" s="12">
         <v>27.1</v>
@@ -1419,16 +1413,16 @@
         <v>375</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="R6" s="34">
         <v>9.2070000000000007</v>
@@ -1441,7 +1435,7 @@
         <v>39.075630252100844</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>3</v>
       </c>
@@ -1449,7 +1443,7 @@
         <v>43676</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" s="12">
         <v>26.6</v>
@@ -1483,16 +1477,16 @@
         <v>375</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="R7" s="34">
         <v>3.34</v>
@@ -1505,7 +1499,7 @@
         <v>14.295497346344803</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>4</v>
       </c>
@@ -1513,7 +1507,7 @@
         <v>43676</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="12">
         <v>20.5</v>
@@ -1548,7 +1542,7 @@
       <c r="S8" s="12"/>
       <c r="T8" s="19"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>5</v>
       </c>
@@ -1556,7 +1550,7 @@
         <v>43676</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D9" s="12">
         <v>30.1</v>
@@ -1590,16 +1584,16 @@
         <v>375</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="R9" s="34">
         <v>3.948</v>
@@ -1612,7 +1606,7 @@
         <v>17.090909090909093</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>6</v>
       </c>
@@ -1620,7 +1614,7 @@
         <v>43676</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D10" s="12">
         <v>36.200000000000003</v>
@@ -1654,16 +1648,16 @@
         <v>375</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="R10" s="34">
         <v>2.2410000000000001</v>
@@ -1676,7 +1670,7 @@
         <v>9.8992843890803091</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>7</v>
       </c>
@@ -1684,7 +1678,7 @@
         <v>43676</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D11" s="12">
         <v>17.100000000000001</v>
@@ -1719,7 +1713,7 @@
       <c r="S11" s="12"/>
       <c r="T11" s="19"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>8</v>
       </c>
@@ -1727,7 +1721,7 @@
         <v>43676</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="12">
         <v>12.5</v>
@@ -1762,7 +1756,7 @@
       <c r="S12" s="12"/>
       <c r="T12" s="19"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="12"/>
@@ -1777,7 +1771,7 @@
       <c r="R13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>1</v>
       </c>
@@ -1785,7 +1779,7 @@
         <v>43690</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" s="12">
         <v>70</v>
@@ -1819,16 +1813,16 @@
         <v>375</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="R14" s="34">
         <v>17.076000000000001</v>
@@ -1841,7 +1835,7 @@
         <v>68.265771168145847</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>2</v>
       </c>
@@ -1849,7 +1843,7 @@
         <v>43690</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="12">
         <v>77.099999999999994</v>
@@ -1883,16 +1877,16 @@
         <v>375</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="R15" s="34">
         <v>19.137</v>
@@ -1905,7 +1899,7 @@
         <v>73.96799628942486</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>3</v>
       </c>
@@ -1913,7 +1907,7 @@
         <v>43690</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" s="12">
         <v>95.1</v>
@@ -1947,16 +1941,16 @@
         <v>375</v>
       </c>
       <c r="N16" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="R16" s="34">
         <v>22.143000000000001</v>
@@ -1969,7 +1963,7 @@
         <v>89.228723404255334</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>4</v>
       </c>
@@ -1977,7 +1971,7 @@
         <v>43690</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D17" s="12">
         <v>84.5</v>
@@ -2011,16 +2005,16 @@
         <v>375</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q17" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="R17" s="34">
         <v>28.091999999999999</v>
@@ -2033,7 +2027,7 @@
         <v>116.29408842523596</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>5</v>
       </c>
@@ -2041,7 +2035,7 @@
         <v>43690</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" s="12">
         <v>81.5</v>
@@ -2075,16 +2069,16 @@
         <v>375</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="R18" s="34">
         <v>29.817</v>
@@ -2097,7 +2091,7 @@
         <v>126.19349923819196</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>6</v>
       </c>
@@ -2105,7 +2099,7 @@
         <v>43690</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" s="12">
         <v>92.3</v>
@@ -2139,16 +2133,16 @@
         <v>375</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q19" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="R19" s="34">
         <v>15.452999999999999</v>
@@ -2161,7 +2155,7 @@
         <v>64.323176823176809</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>7</v>
       </c>
@@ -2169,7 +2163,7 @@
         <v>43690</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D20" s="12">
         <v>99</v>
@@ -2203,16 +2197,16 @@
         <v>375</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="R20" s="34">
         <v>20.616</v>
@@ -2225,7 +2219,7 @@
         <v>79.280110752191959</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>8</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>43690</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D21" s="12">
         <v>78.400000000000006</v>
@@ -2267,16 +2261,16 @@
         <v>375</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q21" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="R21" s="34">
         <v>19.893000000000001</v>
@@ -2289,7 +2283,7 @@
         <v>79.949360983843746</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="C22" s="12"/>
@@ -2304,7 +2298,7 @@
       <c r="R22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>1</v>
       </c>
@@ -2312,7 +2306,7 @@
         <v>43717</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D23" s="12">
         <v>13.6</v>
@@ -2346,16 +2340,16 @@
         <v>375</v>
       </c>
       <c r="N23" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="R23" s="34">
         <v>11.103999999999999</v>
@@ -2368,7 +2362,7 @@
         <v>45.594152911226075</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>2</v>
       </c>
@@ -2376,7 +2370,7 @@
         <v>43717</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D24" s="12">
         <v>16.2</v>
@@ -2410,16 +2404,16 @@
         <v>375</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="R24" s="34">
         <v>2.907</v>
@@ -2432,7 +2426,7 @@
         <v>12.512913223140497</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>3</v>
       </c>
@@ -2440,7 +2434,7 @@
         <v>43717</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D25" s="12">
         <v>22.4</v>
@@ -2474,16 +2468,16 @@
         <v>375</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="R25" s="34">
         <v>5.476</v>
@@ -2496,7 +2490,7 @@
         <v>23.371745625266755</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>4</v>
       </c>
@@ -2504,7 +2498,7 @@
         <v>43717</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D26" s="12">
         <v>21.8</v>
@@ -2538,16 +2532,16 @@
         <v>375</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q26" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="R26" s="34">
         <v>4.4969999999999999</v>
@@ -2560,7 +2554,7 @@
         <v>19.41206941206941</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>5</v>
       </c>
@@ -2568,7 +2562,7 @@
         <v>43717</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D27" s="12">
         <v>25.5</v>
@@ -2602,16 +2596,16 @@
         <v>375</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q27" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="R27" s="34">
         <v>7.3010000000000002</v>
@@ -2624,7 +2618,7 @@
         <v>30.224374896506045</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>6</v>
       </c>
@@ -2632,7 +2626,7 @@
         <v>43717</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28" s="12">
         <v>14.3</v>
@@ -2667,7 +2661,7 @@
       <c r="S28" s="12"/>
       <c r="T28" s="19"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>7</v>
       </c>
@@ -2675,7 +2669,7 @@
         <v>43717</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D29" s="12">
         <v>27.5</v>
@@ -2709,16 +2703,16 @@
         <v>375</v>
       </c>
       <c r="N29" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q29" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q29" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="R29" s="34">
         <v>4.0810000000000004</v>
@@ -2731,7 +2725,7 @@
         <v>17.516525023607176</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>8</v>
       </c>
@@ -2739,7 +2733,7 @@
         <v>43717</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" s="12">
         <v>15</v>
@@ -2774,7 +2768,7 @@
       <c r="S30" s="12"/>
       <c r="T30" s="19"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="12"/>
@@ -2789,7 +2783,7 @@
       <c r="R31" s="5"/>
       <c r="T31" s="5"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>1</v>
       </c>
@@ -2831,16 +2825,16 @@
         <v>375</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O32" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P32" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q32" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="P32" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="R32" s="34">
         <v>4.9390000000000001</v>
@@ -2853,7 +2847,7 @@
         <v>20.844939647168061</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>2</v>
       </c>
@@ -2895,16 +2889,16 @@
         <v>375</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P33" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q33" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="P33" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="R33" s="34">
         <v>8.9909999999999997</v>
@@ -2917,7 +2911,7 @@
         <v>37.425074925074924</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>3</v>
       </c>
@@ -2959,16 +2953,16 @@
         <v>375</v>
       </c>
       <c r="N34" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q34" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="P34" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="R34" s="34">
         <v>6.6390000000000002</v>
@@ -2981,7 +2975,7 @@
         <v>27.787543947764945</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>4</v>
       </c>
@@ -3023,16 +3017,16 @@
         <v>375</v>
       </c>
       <c r="N35" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P35" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q35" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="P35" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="R35" s="34">
         <v>6.6479999999999997</v>
@@ -3045,7 +3039,7 @@
         <v>27.521112767014404</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>5</v>
       </c>
@@ -3087,16 +3081,16 @@
         <v>375</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P36" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q36" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="P36" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="R36" s="34">
         <v>3.629</v>
@@ -3109,7 +3103,7 @@
         <v>16.364538239538241</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>6</v>
       </c>
@@ -3152,7 +3146,7 @@
       <c r="S37" s="12"/>
       <c r="T37" s="19"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>7</v>
       </c>
@@ -3194,16 +3188,16 @@
         <v>375</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="R38" s="34">
         <v>11.289</v>
@@ -3216,7 +3210,7 @@
         <v>48.18181818181818</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>8</v>
       </c>
@@ -3259,7 +3253,7 @@
       <c r="S39" s="12"/>
       <c r="T39" s="19"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="12"/>
@@ -3274,7 +3268,7 @@
       <c r="R40" s="5"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>1</v>
       </c>
@@ -3316,16 +3310,16 @@
         <v>375</v>
       </c>
       <c r="N41" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O41" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q41" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q41" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="R41" s="34">
         <v>9.7579999999999991</v>
@@ -3338,7 +3332,7 @@
         <v>41.069023569023564</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>2</v>
       </c>
@@ -3381,7 +3375,7 @@
       <c r="S42" s="12"/>
       <c r="T42" s="19"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>3</v>
       </c>
@@ -3389,7 +3383,7 @@
         <v>43717</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" s="12">
         <v>13.6</v>
@@ -3424,7 +3418,7 @@
       <c r="S43" s="12"/>
       <c r="T43" s="19"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>4</v>
       </c>
@@ -3466,16 +3460,16 @@
         <v>375</v>
       </c>
       <c r="N44" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O44" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q44" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="R44" s="34">
         <v>7.391</v>
@@ -3488,7 +3482,7 @@
         <v>31.280683934315221</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>5</v>
       </c>
@@ -3496,7 +3490,7 @@
         <v>43717</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45" s="12">
         <v>28.3</v>
@@ -3530,16 +3524,16 @@
         <v>375</v>
       </c>
       <c r="N45" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O45" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q45" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="R45" s="34">
         <v>5.0469999999999997</v>
@@ -3552,7 +3546,7 @@
         <v>21.066032223057015</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>6</v>
       </c>
@@ -3560,7 +3554,7 @@
         <v>43717</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D46" s="12">
         <v>24.1</v>
@@ -3594,16 +3588,16 @@
         <v>375</v>
       </c>
       <c r="N46" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O46" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q46" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="R46" s="34">
         <v>7.3520000000000003</v>
@@ -3616,7 +3610,7 @@
         <v>30.687035645713337</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>7</v>
       </c>
@@ -3624,7 +3618,7 @@
         <v>43717</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47" s="12">
         <v>22.7</v>
@@ -3658,16 +3652,16 @@
         <v>375</v>
       </c>
       <c r="N47" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O47" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q47" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="R47" s="34">
         <v>0.436</v>
@@ -3680,7 +3674,7 @@
         <v>1.8299336858893647</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>8</v>
       </c>
@@ -3688,7 +3682,7 @@
         <v>43717</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" s="12">
         <v>19.8</v>
@@ -3722,16 +3716,16 @@
         <v>375</v>
       </c>
       <c r="N48" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O48" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q48" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="R48" s="34">
         <v>6.5430000000000001</v>
@@ -3744,7 +3738,7 @@
         <v>28.00462249614792</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="12"/>
@@ -3760,7 +3754,7 @@
       <c r="R49" s="5"/>
       <c r="T49" s="5"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="21">
         <v>1</v>
       </c>
@@ -3768,7 +3762,7 @@
         <v>43615</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D50" s="10">
         <v>47.2</v>
@@ -3802,16 +3796,16 @@
         <v>375</v>
       </c>
       <c r="N50" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O50" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q50" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q50" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="R50" s="34">
         <v>0.9234</v>
@@ -3824,7 +3818,7 @@
         <v>4.252555954683614</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="21">
         <v>2</v>
       </c>
@@ -3832,7 +3826,7 @@
         <v>43615</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D51" s="10">
         <v>22.7</v>
@@ -3861,7 +3855,7 @@
       <c r="R51" s="5"/>
       <c r="T51" s="5"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="21">
         <v>3</v>
       </c>
@@ -3869,7 +3863,7 @@
         <v>43615</v>
       </c>
       <c r="C52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D52" s="10">
         <v>31.4</v>
@@ -3903,16 +3897,16 @@
         <v>375</v>
       </c>
       <c r="N52" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O52" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q52" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q52" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="R52" s="34">
         <v>11.484999999999999</v>
@@ -3925,7 +3919,7 @@
         <v>51.030836221452056</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="21">
         <v>4</v>
       </c>
@@ -3933,7 +3927,7 @@
         <v>43615</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D53" s="10">
         <v>30.7</v>
@@ -3968,7 +3962,7 @@
       <c r="S53" s="12"/>
       <c r="T53" s="19"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="9"/>
       <c r="C54" s="12"/>
@@ -3990,7 +3984,7 @@
       <c r="S54" s="12"/>
       <c r="T54" s="19"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="9"/>
       <c r="C55" s="12"/>
@@ -4012,7 +4006,7 @@
       <c r="S55" s="12"/>
       <c r="T55" s="19"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="21">
         <v>1</v>
       </c>
@@ -4020,7 +4014,7 @@
         <v>43622</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" s="10">
         <v>24.2</v>
@@ -4054,16 +4048,16 @@
         <v>375</v>
       </c>
       <c r="N56" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O56" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q56" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="P56" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q56" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="R56" s="34">
         <v>9.3849999999999998</v>
@@ -4076,7 +4070,7 @@
         <v>39.172718924785038</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
         <v>2</v>
       </c>
@@ -4084,7 +4078,7 @@
         <v>43622</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D57" s="10">
         <v>17</v>
@@ -4118,16 +4112,16 @@
         <v>375</v>
       </c>
       <c r="N57" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O57" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q57" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="P57" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q57" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="R57" s="34">
         <v>4.5960000000000001</v>

</xml_diff>